<commit_message>
Build event node graph from excel
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Texts" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Texts (копия)" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Event</t>
   </si>
@@ -31,20 +32,44 @@
     <t>Slavic1</t>
   </si>
   <si>
-    <t>Berimir</t>
-  </si>
-  <si>
-    <t>Какой-то текст</t>
-  </si>
-  <si>
-    <t>Какой-то текст 2</t>
+    <t>Экипаж боевой дружины “Лютик”</t>
+  </si>
+  <si>
+    <t>Гнездо аспидов прямо пред тобой. Надобно уничтожить гадов</t>
+  </si>
+  <si>
+    <t>до</t>
+  </si>
+  <si>
+    <t>Беримир</t>
+  </si>
+  <si>
+    <t>Небыль какая. Ещё же дед сказывал, как перевели они аспидов</t>
+  </si>
+  <si>
+    <t>Темны времена, земли полнятся порождениями, о которых мы и слыхом не слыхивали. Пусть будет верно оружие в бою</t>
+  </si>
+  <si>
+    <t>Беримир отыскал гнездо поганых змеев. Стоило убить одного - приползали десятки. Блестящие шкуры виднелись на сажени вперёд. Он крепче перехватил меч</t>
+  </si>
+  <si>
+    <t>На месте убитых гадов появился чёрный ромб, похожий на камень.</t>
+  </si>
+  <si>
+    <t>после</t>
+  </si>
+  <si>
+    <t>Лютик! Аспиды отправились в тартарары. Дивну невидаль оставили</t>
+  </si>
+  <si>
+    <t>Славна битва твоя. Недалече мужи учёные, растолкуют. Да перестали слово молвить. Поищи, аль не случилось ли чего</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -55,13 +80,35 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF24292F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -70,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -79,6 +126,21 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -89,6 +151,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -317,37 +383,268 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>1.0</v>
       </c>
-      <c r="E2" s="1">
-        <v>-1.0</v>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3">
         <v>1.0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="72.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3">
         <v>1.0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read main plot events from resources
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Texts" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Texts (копия)" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Events" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Texts (копия)" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Event</t>
   </si>
@@ -32,37 +33,61 @@
     <t>Slavic1</t>
   </si>
   <si>
+    <t>Hq</t>
+  </si>
+  <si>
+    <t>Гнездо аспидов прямо пред тобой. Надобно уничтожить гадов</t>
+  </si>
+  <si>
+    <t>Berimir</t>
+  </si>
+  <si>
+    <t>Небыль какая. Ещё же дед сказывал, как перевели они аспидов</t>
+  </si>
+  <si>
+    <t>Темны времена, земли полнятся порождениями, о которых мы и слыхом не слыхивали. Пусть будет верно оружие в бою</t>
+  </si>
+  <si>
+    <t>Беримир отыскал гнездо поганых змеев. Стоило убить одного - приползали десятки. Блестящие шкуры виднелись на сажени вперёд. Он крепче перехватил меч</t>
+  </si>
+  <si>
+    <t>На месте убитых гадов появился чёрный ромб, похожий на камень.</t>
+  </si>
+  <si>
+    <t>Лютик! Аспиды отправились в тартарары. Дивну невидаль оставили</t>
+  </si>
+  <si>
+    <t>Славна битва твоя. Недалече мужи учёные, растолкуют. Да перестали слово молвить. Поищи, аль не случилось ли чего</t>
+  </si>
+  <si>
+    <t>Sid</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Aftermath</t>
+  </si>
+  <si>
+    <t>Глухая чаща</t>
+  </si>
+  <si>
+    <t>Thicket</t>
+  </si>
+  <si>
     <t>Экипаж боевой дружины “Лютик”</t>
   </si>
   <si>
-    <t>Гнездо аспидов прямо пред тобой. Надобно уничтожить гадов</t>
-  </si>
-  <si>
     <t>до</t>
   </si>
   <si>
     <t>Беримир</t>
   </si>
   <si>
-    <t>Небыль какая. Ещё же дед сказывал, как перевели они аспидов</t>
-  </si>
-  <si>
-    <t>Темны времена, земли полнятся порождениями, о которых мы и слыхом не слыхивали. Пусть будет верно оружие в бою</t>
-  </si>
-  <si>
-    <t>Беримир отыскал гнездо поганых змеев. Стоило убить одного - приползали десятки. Блестящие шкуры виднелись на сажени вперёд. Он крепче перехватил меч</t>
-  </si>
-  <si>
-    <t>На месте убитых гадов появился чёрный ромб, похожий на камень.</t>
-  </si>
-  <si>
     <t>после</t>
-  </si>
-  <si>
-    <t>Лютик! Аспиды отправились в тартарары. Дивну невидаль оставили</t>
-  </si>
-  <si>
-    <t>Славна битва твоя. Недалече мужи учёные, растолкуют. Да перестали слово молвить. Поищи, аль не случилось ли чего</t>
   </si>
 </sst>
 </file>
@@ -79,7 +104,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -96,8 +120,9 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +133,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -125,22 +156,22 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -155,6 +186,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -383,118 +418,118 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1.0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>2.0</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
+      <c r="E3" s="3">
+        <v>-1.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
         <v>3.0</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
+      <c r="E4" s="3">
+        <v>-1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
         <v>4.0</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
+      <c r="E5" s="3">
+        <v>-1.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
         <v>1.0</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
+      <c r="E6" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
         <v>2.0</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>14</v>
+      <c r="E7" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2">
         <v>3.0</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
+      <c r="E8" s="3">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -503,6 +538,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -533,118 +608,118 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1.0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2">
         <v>2.0</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2">
         <v>3.0</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3">
-        <v>4.0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
+      <c r="E8" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move The Preying to the after-combat event path + fix game save detection
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\PlotConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C626FD4-DFE9-4465-9F7D-396B9E19A52D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E081058A-88CC-415F-93D4-32FC8D271A26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="325">
   <si>
     <t>Sid</t>
   </si>
@@ -1013,6 +1013,12 @@
   <si>
     <t>Беримир натолько глубоко погружается в молитву, что его невозможно призвать в реальный мир.</t>
   </si>
+  <si>
+    <t>BeforeCombatAftermath</t>
+  </si>
+  <si>
+    <t>AfterCombatAftermath</t>
+  </si>
 </sst>
 </file>
 
@@ -1401,18 +1407,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1423,10 +1431,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1437,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1448,7 +1459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1462,7 +1473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1498,7 +1509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1512,7 +1523,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1523,7 +1534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1537,7 +1548,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1562,7 +1573,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1576,7 +1587,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1590,7 +1601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -1604,7 +1615,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1616,7 +1627,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -1628,7 +1639,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -1642,7 +1653,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1656,7 +1667,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -1670,7 +1681,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
@@ -1692,7 +1703,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
@@ -1703,7 +1714,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>81</v>
       </c>
@@ -1714,7 +1725,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
@@ -1725,7 +1736,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
@@ -1735,7 +1746,7 @@
       <c r="C26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>319</v>
       </c>
     </row>
@@ -1752,7 +1763,7 @@
   </sheetPr>
   <dimension ref="A1:Z1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
@@ -1801,7 +1812,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1839,7 +1850,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +1888,7 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1915,7 +1926,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1951,7 +1962,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -1987,7 +1998,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2025,7 +2036,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -2063,7 +2074,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -2101,7 +2112,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2148,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -2175,7 +2186,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -2211,7 +2222,7 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
@@ -2247,7 +2258,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
@@ -2285,7 +2296,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
@@ -2323,7 +2334,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -2359,7 +2370,7 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
@@ -2397,7 +2408,7 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -2433,7 +2444,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
@@ -2471,7 +2482,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
@@ -2509,7 +2520,7 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
@@ -2547,7 +2558,7 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
@@ -2583,7 +2594,7 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
@@ -2619,7 +2630,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
@@ -2655,7 +2666,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
@@ -2693,7 +2704,7 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
@@ -2731,7 +2742,7 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="6"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>14</v>
       </c>
@@ -2769,7 +2780,7 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>14</v>
       </c>
@@ -2805,7 +2816,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>14</v>
       </c>
@@ -2841,7 +2852,7 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>14</v>
       </c>
@@ -2877,7 +2888,7 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>14</v>
       </c>
@@ -2915,7 +2926,7 @@
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>14</v>
       </c>
@@ -2953,7 +2964,7 @@
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>14</v>
       </c>
@@ -2989,7 +3000,7 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>14</v>
       </c>
@@ -3027,7 +3038,7 @@
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>17</v>
       </c>
@@ -3063,7 +3074,7 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>17</v>
       </c>
@@ -3101,7 +3112,7 @@
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
@@ -32124,7 +32135,7 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -32162,7 +32173,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -32200,7 +32211,7 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -32238,7 +32249,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -32274,7 +32285,7 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
@@ -32310,7 +32321,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -32348,7 +32359,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -32384,7 +32395,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
@@ -32422,7 +32433,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -32460,7 +32471,7 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -32496,7 +32507,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -32534,7 +32545,7 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
@@ -32570,7 +32581,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
@@ -32606,7 +32617,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>7</v>
       </c>
@@ -32642,7 +32653,7 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -32680,7 +32691,7 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>7</v>
       </c>
@@ -32718,7 +32729,7 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
@@ -32754,7 +32765,7 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
@@ -32792,7 +32803,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
@@ -32830,7 +32841,7 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
@@ -32866,7 +32877,7 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
@@ -32904,7 +32915,7 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
@@ -32942,7 +32953,7 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
@@ -32980,7 +32991,7 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
@@ -33018,7 +33029,7 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
@@ -33054,7 +33065,7 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="6"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>10</v>
       </c>
@@ -33092,7 +33103,7 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>10</v>
       </c>
@@ -33128,7 +33139,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>10</v>
       </c>
@@ -33166,7 +33177,7 @@
       <c r="Y29" s="6"/>
       <c r="Z29" s="6"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
@@ -33202,7 +33213,7 @@
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="9"/>
@@ -33230,7 +33241,7 @@
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
@@ -33258,7 +33269,7 @@
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="11"/>
       <c r="C33" s="9"/>
@@ -33286,7 +33297,7 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="11"/>
       <c r="C34" s="9"/>
@@ -33314,7 +33325,7 @@
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="11"/>
       <c r="C35" s="9"/>
@@ -33342,7 +33353,7 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="9"/>
@@ -33370,7 +33381,7 @@
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="8"/>
       <c r="C37" s="9"/>

</xml_diff>

<commit_message>
Display current goal by the plot
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\PlotConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF50E8A0-30FC-48F5-89ED-963EE0B8DB40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736025E6-5009-435F-9563-50C56538CDF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="355">
   <si>
     <t>Sid</t>
   </si>
@@ -1103,6 +1103,12 @@
   <si>
     <t>Другие времена</t>
   </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Найти старый исследовательский центр и спросить учёных про артефакт из моснтра.</t>
+  </si>
 </sst>
 </file>
 
@@ -1203,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1285,6 +1291,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1505,401 +1517,437 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="35" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="36"/>
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="36"/>
+      <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="36"/>
+      <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="36"/>
+      <c r="D12" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="36"/>
+      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="36"/>
+      <c r="D17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="36"/>
+      <c r="D19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="36"/>
+      <c r="D20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="36"/>
+      <c r="D21" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="36"/>
+      <c r="D24" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="36"/>
+      <c r="D25" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>325</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="36"/>
+      <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>330</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="36"/>
+      <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>333</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="36"/>
+      <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>336</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="36"/>
+      <c r="D30" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>345</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="36"/>
+      <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduce parent sids into event's resources
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\PlotConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736025E6-5009-435F-9563-50C56538CDF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D4C8E6-6A8B-4563-BB22-F4CA24386154}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="356">
   <si>
     <t>Sid</t>
   </si>
@@ -1109,6 +1109,9 @@
   <si>
     <t>Найти старый исследовательский центр и спросить учёных про артефакт из моснтра.</t>
   </si>
+  <si>
+    <t>ParentSids</t>
+  </si>
 </sst>
 </file>
 
@@ -1517,10 +1520,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1534,7 @@
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1550,8 +1553,11 @@
       <c r="F1" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1563,7 +1569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1592,7 +1598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1631,7 +1637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1758,7 +1764,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -1771,7 +1777,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -1816,7 +1822,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -1828,7 +1834,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>81</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
@@ -1876,7 +1882,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>87</v>
       </c>
@@ -1890,8 +1896,11 @@
       <c r="F26" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>325</v>
       </c>
@@ -1902,8 +1911,11 @@
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>330</v>
       </c>
@@ -1914,8 +1926,11 @@
       <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>333</v>
       </c>
@@ -1926,8 +1941,11 @@
       <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>336</v>
       </c>
@@ -1938,8 +1956,11 @@
       <c r="D30" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>345</v>
       </c>
@@ -1949,6 +1970,9 @@
       <c r="C31" s="36"/>
       <c r="D31" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix rearranged locations in the demo
</commit_message>
<xml_diff>
--- a/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
+++ b/Rpg.Client/PlotConverter/Ewar - Plot.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="359">
   <si>
     <t>Sid</t>
   </si>
@@ -1007,7 +1007,7 @@
     <t>Возле входа сидит бабушка. Она уже пожила своё, она видела многое. И, честно говоря, её время отличается от теперешнего. Поэтому она просто сидит и безучастно смотрит на всю эту бесполезную суету.</t>
   </si>
   <si>
-    <t>Добраться до болот и выжить.</t>
+    <t>Идти на звук боя.</t>
   </si>
   <si>
     <t>На болотах найти специалиста
@@ -1016,6 +1016,9 @@
   <si>
     <t>В Яме разговорить колдуна.
 Расспросить про корень зла.</t>
+  </si>
+  <si>
+    <t>DestroyedVillage</t>
   </si>
   <si>
     <t>Альфа, приём! Чтоб тебя!</t>
@@ -38441,7 +38444,7 @@
         <v>328</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>17</v>
@@ -38458,7 +38461,7 @@
         <v>329</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>16</v>
+        <v>330</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>24</v>
@@ -38530,7 +38533,7 @@
         <v>110</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D2" s="40">
         <v>1.0</v>
@@ -38568,7 +38571,7 @@
         <v>112</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D3" s="40">
         <v>2.0</v>
@@ -38606,7 +38609,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D4" s="40">
         <v>3.0</v>
@@ -38642,7 +38645,7 @@
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="41" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D5" s="40">
         <v>4.0</v>
@@ -38678,7 +38681,7 @@
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="41" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D6" s="40">
         <v>1.0</v>
@@ -38752,7 +38755,7 @@
       </c>
       <c r="B8" s="44"/>
       <c r="C8" s="41" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D8" s="40">
         <v>2.0</v>
@@ -38790,7 +38793,7 @@
         <v>112</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D9" s="40">
         <v>3.0</v>
@@ -38828,7 +38831,7 @@
         <v>130</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D10" s="40">
         <v>4.0</v>
@@ -38864,7 +38867,7 @@
       </c>
       <c r="B11" s="40"/>
       <c r="C11" s="41" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="40">
         <v>5.0</v>
@@ -38902,7 +38905,7 @@
         <v>130</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D12" s="40">
         <v>6.0</v>
@@ -38938,7 +38941,7 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D13" s="40">
         <v>7.0</v>
@@ -38974,7 +38977,7 @@
       </c>
       <c r="B14" s="43"/>
       <c r="C14" s="41" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D14" s="40">
         <v>1.0</v>
@@ -39010,7 +39013,7 @@
       </c>
       <c r="B15" s="40"/>
       <c r="C15" s="41" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D15" s="40">
         <v>2.0</v>
@@ -39048,7 +39051,7 @@
         <v>112</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D16" s="40">
         <v>3.0</v>
@@ -39086,7 +39089,7 @@
         <v>130</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D17" s="40">
         <v>4.0</v>
@@ -39122,7 +39125,7 @@
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="41" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D18" s="40">
         <v>5.0</v>
@@ -39160,7 +39163,7 @@
         <v>130</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D19" s="40">
         <v>1.0</v>
@@ -39198,7 +39201,7 @@
         <v>150</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D20" s="40">
         <v>2.0</v>
@@ -39234,7 +39237,7 @@
       </c>
       <c r="B21" s="40"/>
       <c r="C21" s="41" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D21" s="40">
         <v>3.0</v>
@@ -39272,7 +39275,7 @@
         <v>150</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D22" s="40">
         <v>4.0</v>
@@ -39310,7 +39313,7 @@
         <v>112</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D23" s="40">
         <v>5.0</v>
@@ -39348,7 +39351,7 @@
         <v>150</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D24" s="40">
         <v>6.0</v>
@@ -39386,7 +39389,7 @@
         <v>130</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D25" s="40">
         <v>7.0</v>
@@ -39422,7 +39425,7 @@
       </c>
       <c r="B26" s="45"/>
       <c r="C26" s="41" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D26" s="40">
         <v>8.0</v>
@@ -39460,7 +39463,7 @@
         <v>112</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D27" s="40">
         <v>1.0</v>
@@ -39496,7 +39499,7 @@
       </c>
       <c r="B28" s="43"/>
       <c r="C28" s="41" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D28" s="40">
         <v>2.0</v>
@@ -39534,7 +39537,7 @@
         <v>130</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D29" s="40">
         <v>3.0</v>
@@ -39570,7 +39573,7 @@
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="41" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D30" s="40">
         <v>4.0</v>

</xml_diff>